<commit_message>
Integrating mapping and grouping variables into updated interface.
</commit_message>
<xml_diff>
--- a/agquery/Update/corr_list.xlsx
+++ b/agquery/Update/corr_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{323AC6FC-62C2-462B-A805-51C9B6606349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EE21E4-DE40-4BCA-A036-9E12EAB9AEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39165" yWindow="2190" windowWidth="29010" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,12 +66,6 @@
     <t>Households that are offered a higher price for their chickens may choose to sell more</t>
   </si>
   <si>
-    <t>contract_coverage_Chickens</t>
-  </si>
-  <si>
-    <t>Households with greater contract coverage may be required to sell their birds</t>
-  </si>
-  <si>
     <t>Egg productivity may be higher if chickens have more room to forage</t>
   </si>
   <si>
@@ -85,6 +79,12 @@
   </si>
   <si>
     <t>Households with more space for chickens may be able to grow their flocks faster</t>
+  </si>
+  <si>
+    <t>yield_Chickens</t>
+  </si>
+  <si>
+    <t>High chicken population density may trigger a sale</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,10 +467,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -481,7 +481,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -492,7 +492,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -503,7 +503,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -514,7 +514,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -525,7 +525,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>